<commit_message>
Added more accurate values
</commit_message>
<xml_diff>
--- a/pyfeng/data/ousv_benchmark.xlsx
+++ b/pyfeng/data/ousv_benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PyFENG\pyfeng\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1499AF-577F-42AC-8150-56EB462BE250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CA05F9-1E46-4E2C-A689-6442FE497BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="743" xr2:uid="{CFD8C97F-677E-4081-BE35-9D7DB797B3CD}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>sigma</t>
   </si>
@@ -105,15 +105,19 @@
   </si>
   <si>
     <t>Table 3 in Li and Wu (2019)</t>
+  </si>
+  <si>
+    <t>Li-Wu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+  <numFmts count="3">
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -152,11 +156,11 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +481,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,152 +525,152 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>0.2</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <f>B2</f>
         <v>0.2</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <v>0.1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>-0.7</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <v>4</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
         <v>100</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="3">
         <v>9.5310000000000006E-2</v>
       </c>
-      <c r="J2" s="3" t="str" cm="1">
+      <c r="J2" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">INDIRECT(A2&amp;"!$B$1")</f>
         <v>Price</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <f t="shared" ref="A3:A5" si="0">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>0.2</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <f>B3</f>
         <v>0.2</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>0.1</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>-0.7</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>4</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>5</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>100</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="3">
         <v>9.5310000000000006E-2</v>
       </c>
-      <c r="J3" s="3" t="str" cm="1">
+      <c r="J3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">INDIRECT(A3&amp;"!$B$1")</f>
         <v>Price</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>0.2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <f>B4</f>
         <v>0.2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>0.1</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>-0.7</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>4</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>10</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>100</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <v>9.5310000000000006E-2</v>
       </c>
-      <c r="J4" s="3" t="str" cm="1">
+      <c r="J4" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">INDIRECT(A4&amp;"!$B$1")</f>
         <v>Price</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>0.25</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>0.25</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>0.3</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>-0.6</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>8</v>
       </c>
-      <c r="G5" s="5">
-        <v>10</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
         <v>100</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="3">
         <v>9.5310000000000006E-2</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -678,7 +682,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5761A8C7-5DBE-4514-94EE-A5933B58C928}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -686,22 +690,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
+        <v>13.214919999999999</v>
+      </c>
+      <c r="C2" s="4">
         <v>13.214930000000001</v>
       </c>
     </row>
@@ -712,25 +723,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FCD568-C350-4F53-ADA8-3A672B89280F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
+        <v>40.797688999999998</v>
+      </c>
+      <c r="C2" s="4">
         <v>40.797730000000001</v>
       </c>
     </row>
@@ -741,27 +762,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F9FDE4-4755-4E32-814A-85CBF4499A47}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
+        <v>62.763120000000001</v>
+      </c>
+      <c r="C2" s="4">
         <v>62.763120000000001</v>
       </c>
     </row>
@@ -772,43 +803,59 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061D7AAA-9DDC-4D37-BE68-08E1503EF93E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>90</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
+        <v>21.418717000000001</v>
+      </c>
+      <c r="C2" s="4">
         <v>21.41873</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>100</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
+        <v>15.16797</v>
+      </c>
+      <c r="C3">
         <v>15.16798</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>110</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
+        <v>10.174469</v>
+      </c>
+      <c r="C4">
         <v>10.174480000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added schobel & zhu examples
</commit_message>
<xml_diff>
--- a/pyfeng/data/ousv_benchmark.xlsx
+++ b/pyfeng/data/ousv_benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PyFENG\pyfeng\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CA05F9-1E46-4E2C-A689-6442FE497BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEF1892-3BDD-4E20-9C62-5502EE9EEC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="743" xr2:uid="{CFD8C97F-677E-4081-BE35-9D7DB797B3CD}"/>
   </bookViews>
@@ -18,6 +18,12 @@
     <sheet name="2" sheetId="32" r:id="rId3"/>
     <sheet name="3" sheetId="31" r:id="rId4"/>
     <sheet name="4" sheetId="33" r:id="rId5"/>
+    <sheet name="5" sheetId="34" r:id="rId6"/>
+    <sheet name="6" sheetId="35" r:id="rId7"/>
+    <sheet name="7" sheetId="36" r:id="rId8"/>
+    <sheet name="8" sheetId="37" r:id="rId9"/>
+    <sheet name="9" sheetId="38" r:id="rId10"/>
+    <sheet name="10" sheetId="39" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>sigma</t>
   </si>
@@ -109,15 +115,51 @@
   <si>
     <t>Li-Wu</t>
   </si>
+  <si>
+    <t>AVBS</t>
+  </si>
+  <si>
+    <t>SSBS</t>
+  </si>
+  <si>
+    <t>Table 1A in Schobel &amp; Zhu (1999)</t>
+  </si>
+  <si>
+    <t>Table 1B in Schobel &amp; Zhu (1999)</t>
+  </si>
+  <si>
+    <t>Table 1C in Schobel &amp; Zhu (1999)</t>
+  </si>
+  <si>
+    <t>Table 2E in Schobel &amp; Zhu (1999)</t>
+  </si>
+  <si>
+    <t>Table 2G in Schobel &amp; Zhu (1999)</t>
+  </si>
+  <si>
+    <t>AVBS-0</t>
+  </si>
+  <si>
+    <t>AVBS-0.1</t>
+  </si>
+  <si>
+    <t>AVBS-0.2</t>
+  </si>
+  <si>
+    <t>AVBS-0.3</t>
+  </si>
+  <si>
+    <t>Table 2D/F in Schobel &amp; Zhu (1999)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -128,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,13 +202,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0584B610-149E-4DFB-B94E-F604CBCB4976}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -539,7 +588,7 @@
       <c r="D2" s="3">
         <v>0.1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>-0.7</v>
       </c>
       <c r="F2" s="3">
@@ -577,7 +626,7 @@
       <c r="D3" s="3">
         <v>0.1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>-0.7</v>
       </c>
       <c r="F3" s="3">
@@ -615,7 +664,7 @@
       <c r="D4" s="3">
         <v>0.1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>-0.7</v>
       </c>
       <c r="F4" s="3">
@@ -652,7 +701,7 @@
       <c r="D5" s="3">
         <v>0.3</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>-0.6</v>
       </c>
       <c r="F5" s="3">
@@ -672,11 +721,687 @@
       </c>
       <c r="K5" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>100</v>
+      </c>
+      <c r="I6" s="3">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>100</v>
+      </c>
+      <c r="I7" s="3">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>100</v>
+      </c>
+      <c r="I8" s="3">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="3">
+        <v>100</v>
+      </c>
+      <c r="I9" s="3">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>100</v>
+      </c>
+      <c r="I10" s="3">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="3">
+        <v>100</v>
+      </c>
+      <c r="I11" s="3">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAD2039-CD05-46C6-AAEA-DBB61BC6455E}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="8.7265625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0.1</v>
+      </c>
+      <c r="E1">
+        <v>0.2</v>
+      </c>
+      <c r="F1">
+        <v>0.3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>90</v>
+      </c>
+      <c r="B2" s="6">
+        <f>C2</f>
+        <v>14.2</v>
+      </c>
+      <c r="C2" s="6">
+        <v>14.2</v>
+      </c>
+      <c r="D2">
+        <v>14.351000000000001</v>
+      </c>
+      <c r="E2">
+        <v>14.871</v>
+      </c>
+      <c r="F2">
+        <v>15.754</v>
+      </c>
+      <c r="G2">
+        <v>14.194000000000001</v>
+      </c>
+      <c r="H2">
+        <v>14.333</v>
+      </c>
+      <c r="I2">
+        <v>14.864000000000001</v>
+      </c>
+      <c r="J2">
+        <v>15.757</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>95</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B8" si="0">C3</f>
+        <v>9.5269999999999992</v>
+      </c>
+      <c r="C3" s="6">
+        <v>9.5269999999999992</v>
+      </c>
+      <c r="D3">
+        <v>9.9969999999999999</v>
+      </c>
+      <c r="E3">
+        <v>10.952</v>
+      </c>
+      <c r="F3">
+        <v>12.198</v>
+      </c>
+      <c r="G3">
+        <v>9.51</v>
+      </c>
+      <c r="H3">
+        <v>9.99</v>
+      </c>
+      <c r="I3">
+        <v>10.962</v>
+      </c>
+      <c r="J3">
+        <v>12.212999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>5.2690000000000001</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5.2690000000000001</v>
+      </c>
+      <c r="D4">
+        <v>6.2539999999999996</v>
+      </c>
+      <c r="E4">
+        <v>7.6319999999999997</v>
+      </c>
+      <c r="F4">
+        <v>9.1609999999999996</v>
+      </c>
+      <c r="G4">
+        <v>5.2770000000000001</v>
+      </c>
+      <c r="H4">
+        <v>6.282</v>
+      </c>
+      <c r="I4">
+        <v>7.6619999999999999</v>
+      </c>
+      <c r="J4">
+        <v>9.1869999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>105</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.17</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2.17</v>
+      </c>
+      <c r="D5">
+        <v>3.4510000000000001</v>
+      </c>
+      <c r="E5">
+        <v>5.0220000000000002</v>
+      </c>
+      <c r="F5">
+        <v>6.6760000000000002</v>
+      </c>
+      <c r="G5">
+        <v>2.2130000000000001</v>
+      </c>
+      <c r="H5">
+        <v>3.4990000000000001</v>
+      </c>
+      <c r="I5">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="J5">
+        <v>6.7069999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>110</v>
+      </c>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="D6">
+        <v>1.679</v>
+      </c>
+      <c r="E6">
+        <v>3.1240000000000001</v>
+      </c>
+      <c r="F6">
+        <v>4.7270000000000003</v>
+      </c>
+      <c r="G6">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="H6">
+        <v>1.708</v>
+      </c>
+      <c r="I6">
+        <v>3.1549999999999998</v>
+      </c>
+      <c r="J6">
+        <v>4.7549999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>115</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D7">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="E7">
+        <v>1.845</v>
+      </c>
+      <c r="F7">
+        <v>3.2589999999999999</v>
+      </c>
+      <c r="G7">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="I7">
+        <v>1.859</v>
+      </c>
+      <c r="J7">
+        <v>3.278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="D8">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="E8">
+        <v>1.04</v>
+      </c>
+      <c r="F8">
+        <v>2.1920000000000002</v>
+      </c>
+      <c r="G8">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="I8">
+        <v>1.0369999999999999</v>
+      </c>
+      <c r="J8">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4B277F-7813-4B15-B237-E2A8BB879385}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="8.7265625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0.1</v>
+      </c>
+      <c r="E1">
+        <v>0.2</v>
+      </c>
+      <c r="F1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>90</v>
+      </c>
+      <c r="B2" s="6">
+        <f>C2</f>
+        <v>14.225</v>
+      </c>
+      <c r="C2" s="6">
+        <v>14.225</v>
+      </c>
+      <c r="D2">
+        <v>14.441000000000001</v>
+      </c>
+      <c r="E2">
+        <v>15.003</v>
+      </c>
+      <c r="F2">
+        <v>15.887</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>95</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B8" si="0">C3</f>
+        <v>9.6</v>
+      </c>
+      <c r="C3" s="6">
+        <v>9.6</v>
+      </c>
+      <c r="D3">
+        <v>10.130000000000001</v>
+      </c>
+      <c r="E3">
+        <v>11.084</v>
+      </c>
+      <c r="F3">
+        <v>12.305999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>5.3719999999999999</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5.3719999999999999</v>
+      </c>
+      <c r="D4">
+        <v>6.3609999999999998</v>
+      </c>
+      <c r="E4">
+        <v>7.71</v>
+      </c>
+      <c r="F4">
+        <v>9.2129999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>105</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1520000000000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2.1520000000000001</v>
+      </c>
+      <c r="D5">
+        <v>3.4350000000000001</v>
+      </c>
+      <c r="E5">
+        <v>5.0030000000000001</v>
+      </c>
+      <c r="F5">
+        <v>6.6520000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>110</v>
+      </c>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.504</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.504</v>
+      </c>
+      <c r="D6">
+        <v>1.5289999999999999</v>
+      </c>
+      <c r="E6">
+        <v>3.004</v>
+      </c>
+      <c r="F6">
+        <v>4.6260000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>115</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="E7">
+        <v>1.66</v>
+      </c>
+      <c r="F7">
+        <v>3.097</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C8" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D8">
+        <v>0.155</v>
+      </c>
+      <c r="E8">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="F8">
+        <v>1.9950000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -862,4 +1587,1203 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6B2DAA-FB44-4708-96F6-DD88B104329D}">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" activeCellId="1" sqref="B1:B1048576 I1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.7265625" style="6"/>
+    <col min="9" max="9" width="8.7265625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1">
+        <v>-1</v>
+      </c>
+      <c r="F1">
+        <v>-0.75</v>
+      </c>
+      <c r="G1">
+        <v>-0.5</v>
+      </c>
+      <c r="H1">
+        <v>-0.25</v>
+      </c>
+      <c r="I1" s="6">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0.25</v>
+      </c>
+      <c r="K1">
+        <v>0.5</v>
+      </c>
+      <c r="L1">
+        <v>0.75</v>
+      </c>
+      <c r="M1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>90</v>
+      </c>
+      <c r="B2" s="6">
+        <f>I2</f>
+        <v>15.154999999999999</v>
+      </c>
+      <c r="C2">
+        <v>15.151999999999999</v>
+      </c>
+      <c r="D2">
+        <v>15.118</v>
+      </c>
+      <c r="E2">
+        <v>15.416</v>
+      </c>
+      <c r="F2">
+        <v>15.355</v>
+      </c>
+      <c r="G2">
+        <v>15.292</v>
+      </c>
+      <c r="H2">
+        <v>15.225</v>
+      </c>
+      <c r="I2" s="6">
+        <v>15.154999999999999</v>
+      </c>
+      <c r="J2">
+        <v>15.081</v>
+      </c>
+      <c r="K2">
+        <v>15.003</v>
+      </c>
+      <c r="L2">
+        <v>14.919</v>
+      </c>
+      <c r="M2">
+        <v>14.827999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>95</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B8" si="0">I3</f>
+        <v>11.379</v>
+      </c>
+      <c r="C3">
+        <v>11.391</v>
+      </c>
+      <c r="D3">
+        <v>11.342000000000001</v>
+      </c>
+      <c r="E3">
+        <v>11.617000000000001</v>
+      </c>
+      <c r="F3">
+        <v>11.561999999999999</v>
+      </c>
+      <c r="G3">
+        <v>11.503</v>
+      </c>
+      <c r="H3">
+        <v>11.443</v>
+      </c>
+      <c r="I3" s="6">
+        <v>11.379</v>
+      </c>
+      <c r="J3">
+        <v>11.313000000000001</v>
+      </c>
+      <c r="K3">
+        <v>11.243</v>
+      </c>
+      <c r="L3">
+        <v>11.169</v>
+      </c>
+      <c r="M3">
+        <v>11.092000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>8.1760000000000002</v>
+      </c>
+      <c r="C4">
+        <v>8.2029999999999994</v>
+      </c>
+      <c r="D4">
+        <v>8.1419999999999995</v>
+      </c>
+      <c r="E4">
+        <v>8.3070000000000004</v>
+      </c>
+      <c r="F4">
+        <v>8.2750000000000004</v>
+      </c>
+      <c r="G4">
+        <v>8.2430000000000003</v>
+      </c>
+      <c r="H4">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="I4" s="6">
+        <v>8.1760000000000002</v>
+      </c>
+      <c r="J4">
+        <v>8.141</v>
+      </c>
+      <c r="K4">
+        <v>8.1059999999999999</v>
+      </c>
+      <c r="L4">
+        <v>8.07</v>
+      </c>
+      <c r="M4">
+        <v>8.0340000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>105</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>5.617</v>
+      </c>
+      <c r="C5">
+        <v>5.65</v>
+      </c>
+      <c r="D5">
+        <v>5.5839999999999996</v>
+      </c>
+      <c r="E5">
+        <v>5.5759999999999996</v>
+      </c>
+      <c r="F5">
+        <v>5.585</v>
+      </c>
+      <c r="G5">
+        <v>5.5949999999999998</v>
+      </c>
+      <c r="H5">
+        <v>5.6059999999999999</v>
+      </c>
+      <c r="I5" s="6">
+        <v>5.617</v>
+      </c>
+      <c r="J5">
+        <v>5.6280000000000001</v>
+      </c>
+      <c r="K5">
+        <v>5.64</v>
+      </c>
+      <c r="L5">
+        <v>5.6520000000000001</v>
+      </c>
+      <c r="M5">
+        <v>5.665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>110</v>
+      </c>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>3.694</v>
+      </c>
+      <c r="C6">
+        <v>3.722</v>
+      </c>
+      <c r="D6">
+        <v>3.6579999999999999</v>
+      </c>
+      <c r="E6">
+        <v>3.468</v>
+      </c>
+      <c r="F6">
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="G6">
+        <v>3.5819999999999999</v>
+      </c>
+      <c r="H6">
+        <v>3.6379999999999999</v>
+      </c>
+      <c r="I6" s="6">
+        <v>3.694</v>
+      </c>
+      <c r="J6">
+        <v>3.7490000000000001</v>
+      </c>
+      <c r="K6">
+        <v>3.8029999999999999</v>
+      </c>
+      <c r="L6">
+        <v>3.8559999999999999</v>
+      </c>
+      <c r="M6">
+        <v>3.9089999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>115</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>2.3330000000000002</v>
+      </c>
+      <c r="C7">
+        <v>2.3490000000000002</v>
+      </c>
+      <c r="D7">
+        <v>2.2930000000000001</v>
+      </c>
+      <c r="E7">
+        <v>1.966</v>
+      </c>
+      <c r="F7">
+        <v>2.0630000000000002</v>
+      </c>
+      <c r="G7">
+        <v>2.1560000000000001</v>
+      </c>
+      <c r="H7">
+        <v>2.246</v>
+      </c>
+      <c r="I7" s="6">
+        <v>2.3330000000000002</v>
+      </c>
+      <c r="J7">
+        <v>2.4159999999999999</v>
+      </c>
+      <c r="K7">
+        <v>2.4969999999999999</v>
+      </c>
+      <c r="L7">
+        <v>2.5760000000000001</v>
+      </c>
+      <c r="M7">
+        <v>2.653</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>1.42</v>
+      </c>
+      <c r="C8">
+        <v>1.4219999999999999</v>
+      </c>
+      <c r="D8">
+        <v>1.377</v>
+      </c>
+      <c r="E8">
+        <v>0.995</v>
+      </c>
+      <c r="F8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G8">
+        <v>1.218</v>
+      </c>
+      <c r="H8">
+        <v>1.321</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1.42</v>
+      </c>
+      <c r="J8">
+        <v>1.514</v>
+      </c>
+      <c r="K8">
+        <v>1.605</v>
+      </c>
+      <c r="L8">
+        <v>1.6930000000000001</v>
+      </c>
+      <c r="M8">
+        <v>1.7769999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE24A2D-D7B0-4647-B24E-987FE01149C0}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" activeCellId="1" sqref="B1:B1048576 H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.7265625" style="6"/>
+    <col min="8" max="8" width="8.7265625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1">
+        <v>-1</v>
+      </c>
+      <c r="E1">
+        <v>-0.75</v>
+      </c>
+      <c r="F1">
+        <v>-0.5</v>
+      </c>
+      <c r="G1">
+        <v>-0.25</v>
+      </c>
+      <c r="H1" s="6">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0.25</v>
+      </c>
+      <c r="J1">
+        <v>0.5</v>
+      </c>
+      <c r="K1">
+        <v>0.75</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>90</v>
+      </c>
+      <c r="B2" s="6">
+        <f>H2</f>
+        <v>14.515000000000001</v>
+      </c>
+      <c r="C2">
+        <v>14.500999999999999</v>
+      </c>
+      <c r="D2">
+        <v>14.73</v>
+      </c>
+      <c r="E2">
+        <v>14.679</v>
+      </c>
+      <c r="F2">
+        <v>14.625999999999999</v>
+      </c>
+      <c r="G2">
+        <v>14.571999999999999</v>
+      </c>
+      <c r="H2" s="6">
+        <v>14.515000000000001</v>
+      </c>
+      <c r="I2">
+        <v>14.456</v>
+      </c>
+      <c r="J2">
+        <v>14.395</v>
+      </c>
+      <c r="K2">
+        <v>14.33</v>
+      </c>
+      <c r="L2">
+        <v>14.260999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>95</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B8" si="0">H3</f>
+        <v>10.346</v>
+      </c>
+      <c r="C3">
+        <v>10.348000000000001</v>
+      </c>
+      <c r="D3">
+        <v>10.6</v>
+      </c>
+      <c r="E3">
+        <v>10.541</v>
+      </c>
+      <c r="F3">
+        <v>10.48</v>
+      </c>
+      <c r="G3">
+        <v>10.414999999999999</v>
+      </c>
+      <c r="H3" s="6">
+        <v>10.346</v>
+      </c>
+      <c r="I3">
+        <v>10.271000000000001</v>
+      </c>
+      <c r="J3">
+        <v>10.191000000000001</v>
+      </c>
+      <c r="K3">
+        <v>10.103</v>
+      </c>
+      <c r="L3">
+        <v>10.005000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>6.8029999999999999</v>
+      </c>
+      <c r="C4">
+        <v>6.8289999999999997</v>
+      </c>
+      <c r="D4">
+        <v>6.976</v>
+      </c>
+      <c r="E4">
+        <v>6.9359999999999999</v>
+      </c>
+      <c r="F4">
+        <v>6.8940000000000001</v>
+      </c>
+      <c r="G4">
+        <v>6.8490000000000002</v>
+      </c>
+      <c r="H4" s="6">
+        <v>6.8029999999999999</v>
+      </c>
+      <c r="I4">
+        <v>6.7530000000000001</v>
+      </c>
+      <c r="J4">
+        <v>6.7009999999999996</v>
+      </c>
+      <c r="K4">
+        <v>6.6449999999999996</v>
+      </c>
+      <c r="L4">
+        <v>6.5869999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>105</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>4.093</v>
+      </c>
+      <c r="C5">
+        <v>4.1319999999999997</v>
+      </c>
+      <c r="D5">
+        <v>4.0570000000000004</v>
+      </c>
+      <c r="E5">
+        <v>4.0659999999999998</v>
+      </c>
+      <c r="F5">
+        <v>4.0750000000000002</v>
+      </c>
+      <c r="G5">
+        <v>4.085</v>
+      </c>
+      <c r="H5" s="6">
+        <v>4.093</v>
+      </c>
+      <c r="I5">
+        <v>4.1020000000000003</v>
+      </c>
+      <c r="J5">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="K5">
+        <v>4.117</v>
+      </c>
+      <c r="L5">
+        <v>4.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>110</v>
+      </c>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>2.254</v>
+      </c>
+      <c r="C6">
+        <v>2.282</v>
+      </c>
+      <c r="D6">
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="E6">
+        <v>2.0510000000000002</v>
+      </c>
+      <c r="F6">
+        <v>2.121</v>
+      </c>
+      <c r="G6">
+        <v>2.1890000000000001</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2.254</v>
+      </c>
+      <c r="I6">
+        <v>2.3159999999999998</v>
+      </c>
+      <c r="J6">
+        <v>2.3759999999999999</v>
+      </c>
+      <c r="K6">
+        <v>2.4329999999999998</v>
+      </c>
+      <c r="L6">
+        <v>2.4889999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>115</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="C7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="F7">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="G7">
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="I7">
+        <v>1.23</v>
+      </c>
+      <c r="J7">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="K7">
+        <v>1.389</v>
+      </c>
+      <c r="L7">
+        <v>1.4630000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="C8">
+        <v>0.53</v>
+      </c>
+      <c r="D8">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="F8">
+        <v>0.371</v>
+      </c>
+      <c r="G8">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="I8">
+        <v>0.621</v>
+      </c>
+      <c r="J8">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="K8">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="L8">
+        <v>0.84499999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F9FD47-1490-4478-A2C0-1F2C85519101}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.7265625" style="6"/>
+    <col min="8" max="8" width="8.7265625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1">
+        <v>-1</v>
+      </c>
+      <c r="E1">
+        <v>-0.75</v>
+      </c>
+      <c r="F1">
+        <v>-0.5</v>
+      </c>
+      <c r="G1">
+        <v>-0.25</v>
+      </c>
+      <c r="H1" s="6">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0.25</v>
+      </c>
+      <c r="J1">
+        <v>0.5</v>
+      </c>
+      <c r="K1">
+        <v>0.75</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>90</v>
+      </c>
+      <c r="B2" s="6">
+        <f>H2</f>
+        <v>16.106000000000002</v>
+      </c>
+      <c r="C2">
+        <v>16.111000000000001</v>
+      </c>
+      <c r="D2">
+        <v>16.356999999999999</v>
+      </c>
+      <c r="E2">
+        <v>16.297999999999998</v>
+      </c>
+      <c r="F2">
+        <v>16.236000000000001</v>
+      </c>
+      <c r="G2">
+        <v>16.172000000000001</v>
+      </c>
+      <c r="H2" s="6">
+        <v>16.106000000000002</v>
+      </c>
+      <c r="I2">
+        <v>16.036999999999999</v>
+      </c>
+      <c r="J2">
+        <v>15.964</v>
+      </c>
+      <c r="K2">
+        <v>15.888999999999999</v>
+      </c>
+      <c r="L2">
+        <v>15.81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>95</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B8" si="0">H3</f>
+        <v>12.651</v>
+      </c>
+      <c r="C3">
+        <v>12.666</v>
+      </c>
+      <c r="D3">
+        <v>12.846</v>
+      </c>
+      <c r="E3">
+        <v>12.8</v>
+      </c>
+      <c r="F3">
+        <v>12.750999999999999</v>
+      </c>
+      <c r="G3">
+        <v>12.702</v>
+      </c>
+      <c r="H3" s="6">
+        <v>12.651</v>
+      </c>
+      <c r="I3">
+        <v>12.598000000000001</v>
+      </c>
+      <c r="J3">
+        <v>12.544</v>
+      </c>
+      <c r="K3">
+        <v>12.489000000000001</v>
+      </c>
+      <c r="L3">
+        <v>12.432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>9.6869999999999994</v>
+      </c>
+      <c r="C4">
+        <v>9.7110000000000003</v>
+      </c>
+      <c r="D4">
+        <v>9.7769999999999992</v>
+      </c>
+      <c r="E4">
+        <v>9.7550000000000008</v>
+      </c>
+      <c r="F4">
+        <v>9.7319999999999993</v>
+      </c>
+      <c r="G4">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="H4" s="6">
+        <v>9.6869999999999994</v>
+      </c>
+      <c r="I4">
+        <v>9.6649999999999991</v>
+      </c>
+      <c r="J4">
+        <v>9.6419999999999995</v>
+      </c>
+      <c r="K4">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="L4">
+        <v>9.5980000000000008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>105</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>7.2370000000000001</v>
+      </c>
+      <c r="C5">
+        <v>7.2640000000000002</v>
+      </c>
+      <c r="D5">
+        <v>7.1859999999999999</v>
+      </c>
+      <c r="E5">
+        <v>7.1980000000000004</v>
+      </c>
+      <c r="F5">
+        <v>7.21</v>
+      </c>
+      <c r="G5">
+        <v>7.2229999999999999</v>
+      </c>
+      <c r="H5" s="6">
+        <v>7.2370000000000001</v>
+      </c>
+      <c r="I5">
+        <v>7.2510000000000003</v>
+      </c>
+      <c r="J5">
+        <v>7.2649999999999997</v>
+      </c>
+      <c r="K5">
+        <v>7.28</v>
+      </c>
+      <c r="L5">
+        <v>7.2960000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>110</v>
+      </c>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>5.2789999999999999</v>
+      </c>
+      <c r="C6">
+        <v>5.3049999999999997</v>
+      </c>
+      <c r="D6">
+        <v>5.0839999999999996</v>
+      </c>
+      <c r="E6">
+        <v>5.133</v>
+      </c>
+      <c r="F6">
+        <v>5.1820000000000004</v>
+      </c>
+      <c r="G6">
+        <v>5.23</v>
+      </c>
+      <c r="H6" s="6">
+        <v>5.2789999999999999</v>
+      </c>
+      <c r="I6">
+        <v>5.3280000000000003</v>
+      </c>
+      <c r="J6">
+        <v>5.3769999999999998</v>
+      </c>
+      <c r="K6">
+        <v>5.4260000000000002</v>
+      </c>
+      <c r="L6">
+        <v>5.4749999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>115</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7679999999999998</v>
+      </c>
+      <c r="C7">
+        <v>3.786</v>
+      </c>
+      <c r="D7">
+        <v>3.4489999999999998</v>
+      </c>
+      <c r="E7">
+        <v>3.5310000000000001</v>
+      </c>
+      <c r="F7">
+        <v>3.6110000000000002</v>
+      </c>
+      <c r="G7">
+        <v>3.69</v>
+      </c>
+      <c r="H7" s="6">
+        <v>3.7679999999999998</v>
+      </c>
+      <c r="I7">
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="J7">
+        <v>3.919</v>
+      </c>
+      <c r="K7">
+        <v>3.9929999999999999</v>
+      </c>
+      <c r="L7">
+        <v>4.0650000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>2.6349999999999998</v>
+      </c>
+      <c r="C8">
+        <v>2.6459999999999999</v>
+      </c>
+      <c r="D8">
+        <v>2.2349999999999999</v>
+      </c>
+      <c r="E8">
+        <v>2.34</v>
+      </c>
+      <c r="F8">
+        <v>2.4409999999999998</v>
+      </c>
+      <c r="G8">
+        <v>2.54</v>
+      </c>
+      <c r="H8" s="6">
+        <v>2.6349999999999998</v>
+      </c>
+      <c r="I8">
+        <v>2.7280000000000002</v>
+      </c>
+      <c r="J8">
+        <v>2.819</v>
+      </c>
+      <c r="K8">
+        <v>2.9079999999999999</v>
+      </c>
+      <c r="L8">
+        <v>2.9940000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDE6EBC-20C5-4C4A-8F41-F3804F8029F0}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="8.7265625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0.1</v>
+      </c>
+      <c r="E1">
+        <v>0.2</v>
+      </c>
+      <c r="F1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>90</v>
+      </c>
+      <c r="B2" s="6">
+        <f>C2</f>
+        <v>14.189</v>
+      </c>
+      <c r="C2" s="6">
+        <v>14.189</v>
+      </c>
+      <c r="D2">
+        <v>14.262</v>
+      </c>
+      <c r="E2">
+        <v>14.723000000000001</v>
+      </c>
+      <c r="F2">
+        <v>15.608000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>95</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B8" si="0">C3</f>
+        <v>9.4589999999999996</v>
+      </c>
+      <c r="C3" s="6">
+        <v>9.4589999999999996</v>
+      </c>
+      <c r="D3">
+        <v>9.8420000000000005</v>
+      </c>
+      <c r="E3">
+        <v>10.804</v>
+      </c>
+      <c r="F3">
+        <v>12.082000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>5.141</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5.141</v>
+      </c>
+      <c r="D4">
+        <v>6.1319999999999997</v>
+      </c>
+      <c r="E4">
+        <v>7.5510000000000002</v>
+      </c>
+      <c r="F4">
+        <v>9.109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>105</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.173</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2.173</v>
+      </c>
+      <c r="D5">
+        <v>3.4660000000000002</v>
+      </c>
+      <c r="E5">
+        <v>5.0439999999999996</v>
+      </c>
+      <c r="F5">
+        <v>6.7030000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>110</v>
+      </c>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="D6">
+        <v>1.8120000000000001</v>
+      </c>
+      <c r="E6">
+        <v>3.2389999999999999</v>
+      </c>
+      <c r="F6">
+        <v>4.8280000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>115</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E7">
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="F7">
+        <v>3.4140000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C8" s="6">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E8">
+        <v>1.22</v>
+      </c>
+      <c r="F8">
+        <v>2.3759999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>